<commit_message>
Updated app layout and example config
</commit_message>
<xml_diff>
--- a/interaction_config.xlsx
+++ b/interaction_config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccireland-my.sharepoint.com/personal/nsoledadrioscolombo_ucc_ie/Documents/Natalia Rios/Experiments/SIHUMI Network Model/SIHUMI/Open_Source_Version/Python_ver/MICRONETPLOT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccireland-my.sharepoint.com/personal/nsoledadrioscolombo_ucc_ie/Documents/Natalia Rios/Experiments/SIHUMI Network Model/SIHUMI/Open_Source_Version/Python_ver/micronet_app_v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="11_F25DC773A252ABDACC1048EFA19E68BE5ADE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B53E4819-827B-4A8D-9C71-CB9CC0D4718E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ED1C126-E095-4B7D-87BF-6789476A9FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>B. longum</t>
   </si>
@@ -64,41 +64,65 @@
     <t>C.difficile</t>
   </si>
   <si>
-    <t>restfactor</t>
-  </si>
-  <si>
-    <t>linewidth_base</t>
-  </si>
-  <si>
-    <t>linewidth_scale</t>
-  </si>
-  <si>
-    <t>arrowsize_base</t>
-  </si>
-  <si>
-    <t>arrowsize_scale</t>
-  </si>
-  <si>
     <t>nodeFontSize</t>
   </si>
   <si>
     <t>C. scindens</t>
   </si>
   <si>
-    <t>combined_alpha</t>
-  </si>
-  <si>
-    <t>minconflag</t>
-  </si>
-  <si>
-    <t>neutral_strength</t>
+    <t>scale neutral strength</t>
+  </si>
+  <si>
+    <t>scale linewidth</t>
+  </si>
+  <si>
+    <t>scale arrowsize</t>
+  </si>
+  <si>
+    <t>combined transparency</t>
+  </si>
+  <si>
+    <t>nodeSize</t>
+  </si>
+  <si>
+    <t>nodeColor</t>
+  </si>
+  <si>
+    <t>#00FF00</t>
+  </si>
+  <si>
+    <t>Positive Line Color</t>
+  </si>
+  <si>
+    <t>Negative Line Color</t>
+  </si>
+  <si>
+    <t>Positive Arrow Color</t>
+  </si>
+  <si>
+    <t>Negative Arrow Color</t>
+  </si>
+  <si>
+    <t>#6E9E9E</t>
+  </si>
+  <si>
+    <t>#F5C159</t>
+  </si>
+  <si>
+    <t>#587E8B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #D98B4B</t>
+  </si>
+  <si>
+    <t>Neutral Color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +143,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -149,6 +178,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,10 +200,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,9 +471,9 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="45">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -468,10 +500,10 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -503,7 +535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="45">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -535,7 +567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -567,7 +599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="45">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -599,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="30">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -631,7 +663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -663,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="30">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -695,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="30">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -727,9 +759,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -772,9 +804,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="45">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -801,10 +833,10 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -836,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="45">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -868,7 +900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -900,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="45">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -932,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="30">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -964,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -996,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="30">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="30">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1060,9 +1092,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -1100,89 +1132,147 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30C8B70-53F8-4C31-B528-9EE08736CD68}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="B5" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>